<commit_message>
SIMPLEX-114 Enforce translation's language code.
</commit_message>
<xml_diff>
--- a/api/src/test/resources/test-spreadsheets/conceptsSpreadsheet-blank-term.xlsx
+++ b/api/src/test/resources/test-spreadsheets/conceptsSpreadsheet-blank-term.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/c/simple-extension-toolkit/api/src/test/resources/test-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3E561F-D7AD-824D-884F-BCA25A8F084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7E8928-58E2-3648-A01E-5C39D9FC68DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -159,39 +159,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Terms in English, US dialect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The first term will be the preferred term. _x000D_
-Each additional synonym should use a new row. There is no need to repeat the values in columns A to D.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Terms in My translation (214916581000003106)</t>
     </r>
     <r>
@@ -353,6 +320,29 @@
   </si>
   <si>
     <t>Simplex branch timestamp:1727964880378</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Terms in English, US dialect. This term is required.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The first term will be the preferred term. 
+Each additional synonym should use a new row. There is no need to repeat the values in columns A to D.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -739,7 +729,7 @@
   <dimension ref="A1:CA15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,286 +755,286 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="CA1" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:79" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:79" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>